<commit_message>
updated timeline and details with bartlett and underc, and u_mich_bio has been removed from the sites
</commit_message>
<xml_diff>
--- a/snow_timeline.xlsx
+++ b/snow_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A54B1C3-3F45-4589-B0FC-AFAD735E5BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1705EC-1B27-4D1B-AFE7-24D28A843343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="492" windowWidth="23040" windowHeight="12240" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
+    <workbookView xWindow="5868" yWindow="372" windowWidth="17280" windowHeight="9960" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="13">
   <si>
     <t>Location</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>underc</t>
+  </si>
+  <si>
+    <t>bartlett</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0BDC52-0678-4879-BFA4-045E88D6C76C}">
-  <dimension ref="A1:D1087"/>
+  <dimension ref="A1:D1203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1064" workbookViewId="0">
-      <selection activeCell="A1075" sqref="A1075:A1087"/>
+    <sheetView tabSelected="1" topLeftCell="A1177" workbookViewId="0">
+      <selection activeCell="D1193" sqref="D1193:D1203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14740,13 +14743,13 @@
         <v>4</v>
       </c>
       <c r="B1020" s="1">
-        <v>43231</v>
+        <v>44328</v>
       </c>
       <c r="C1020">
         <v>100</v>
       </c>
       <c r="D1020">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1021" spans="1:4" x14ac:dyDescent="0.3">
@@ -14754,13 +14757,13 @@
         <v>4</v>
       </c>
       <c r="B1021" s="1">
-        <v>43232</v>
+        <v>44329</v>
       </c>
       <c r="C1021">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1021">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1022" spans="1:4" x14ac:dyDescent="0.3">
@@ -14768,13 +14771,14 @@
         <v>4</v>
       </c>
       <c r="B1022" s="1">
-        <v>43233</v>
+        <v>44330</v>
       </c>
       <c r="C1022">
-        <v>99</v>
+        <f>C1021-1/4</f>
+        <v>99.75</v>
       </c>
       <c r="D1022">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1023" spans="1:4" x14ac:dyDescent="0.3">
@@ -14782,13 +14786,14 @@
         <v>4</v>
       </c>
       <c r="B1023" s="1">
-        <v>43234</v>
+        <v>44331</v>
       </c>
       <c r="C1023">
-        <v>98</v>
+        <f t="shared" ref="C1023:C1024" si="13">C1022-1/4</f>
+        <v>99.5</v>
       </c>
       <c r="D1023">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1024" spans="1:4" x14ac:dyDescent="0.3">
@@ -14796,13 +14801,14 @@
         <v>4</v>
       </c>
       <c r="B1024" s="1">
-        <v>43235</v>
+        <v>44332</v>
       </c>
       <c r="C1024">
-        <v>97</v>
+        <f t="shared" si="13"/>
+        <v>99.25</v>
       </c>
       <c r="D1024">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1025" spans="1:4" x14ac:dyDescent="0.3">
@@ -14810,13 +14816,13 @@
         <v>4</v>
       </c>
       <c r="B1025" s="1">
-        <v>43236</v>
+        <v>44333</v>
       </c>
       <c r="C1025">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D1025">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1026" spans="1:4" x14ac:dyDescent="0.3">
@@ -14824,13 +14830,14 @@
         <v>4</v>
       </c>
       <c r="B1026" s="1">
-        <v>43237</v>
+        <v>44334</v>
       </c>
       <c r="C1026">
-        <v>95</v>
+        <f>C1025-2/3</f>
+        <v>98.333333333333329</v>
       </c>
       <c r="D1026">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1027" spans="1:4" x14ac:dyDescent="0.3">
@@ -14838,13 +14845,14 @@
         <v>4</v>
       </c>
       <c r="B1027" s="1">
-        <v>43238</v>
+        <v>44335</v>
       </c>
       <c r="C1027">
-        <v>93</v>
+        <f>C1026-2/3</f>
+        <v>97.666666666666657</v>
       </c>
       <c r="D1027">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1028" spans="1:4" x14ac:dyDescent="0.3">
@@ -14852,13 +14860,13 @@
         <v>4</v>
       </c>
       <c r="B1028" s="1">
-        <v>43239</v>
+        <v>44336</v>
       </c>
       <c r="C1028">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D1028">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1029" spans="1:4" x14ac:dyDescent="0.3">
@@ -14866,13 +14874,13 @@
         <v>4</v>
       </c>
       <c r="B1029" s="1">
-        <v>43240</v>
+        <v>44337</v>
       </c>
       <c r="C1029">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D1029">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1030" spans="1:4" x14ac:dyDescent="0.3">
@@ -14880,13 +14888,13 @@
         <v>4</v>
       </c>
       <c r="B1030" s="1">
-        <v>43241</v>
+        <v>44338</v>
       </c>
       <c r="C1030">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D1030">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1031" spans="1:4" x14ac:dyDescent="0.3">
@@ -14894,13 +14902,13 @@
         <v>4</v>
       </c>
       <c r="B1031" s="1">
-        <v>43242</v>
+        <v>44339</v>
       </c>
       <c r="C1031">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D1031">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1032" spans="1:4" x14ac:dyDescent="0.3">
@@ -14908,13 +14916,13 @@
         <v>4</v>
       </c>
       <c r="B1032" s="1">
-        <v>43243</v>
+        <v>44340</v>
       </c>
       <c r="C1032">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D1032">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1033" spans="1:4" x14ac:dyDescent="0.3">
@@ -14922,13 +14930,13 @@
         <v>4</v>
       </c>
       <c r="B1033" s="1">
-        <v>43244</v>
+        <v>44341</v>
       </c>
       <c r="C1033">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D1033">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1034" spans="1:4" x14ac:dyDescent="0.3">
@@ -14936,13 +14944,13 @@
         <v>4</v>
       </c>
       <c r="B1034" s="1">
-        <v>43245</v>
+        <v>44342</v>
       </c>
       <c r="C1034">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D1034">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1035" spans="1:4" x14ac:dyDescent="0.3">
@@ -14950,13 +14958,14 @@
         <v>4</v>
       </c>
       <c r="B1035" s="1">
-        <v>43246</v>
+        <v>44343</v>
       </c>
       <c r="C1035">
-        <v>75</v>
+        <f>C1034-11/2</f>
+        <v>85.5</v>
       </c>
       <c r="D1035">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1036" spans="1:4" x14ac:dyDescent="0.3">
@@ -14964,13 +14973,13 @@
         <v>4</v>
       </c>
       <c r="B1036" s="1">
-        <v>43247</v>
+        <v>44344</v>
       </c>
       <c r="C1036">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D1036">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1037" spans="1:4" x14ac:dyDescent="0.3">
@@ -14978,13 +14987,14 @@
         <v>4</v>
       </c>
       <c r="B1037" s="1">
-        <v>43248</v>
+        <v>44345</v>
       </c>
       <c r="C1037">
-        <v>63</v>
+        <f>C1036-24/3</f>
+        <v>72</v>
       </c>
       <c r="D1037">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1038" spans="1:4" x14ac:dyDescent="0.3">
@@ -14992,13 +15002,14 @@
         <v>4</v>
       </c>
       <c r="B1038" s="1">
-        <v>43249</v>
+        <v>44346</v>
       </c>
       <c r="C1038">
-        <v>55</v>
+        <f>C1037-24/3</f>
+        <v>64</v>
       </c>
       <c r="D1038">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1039" spans="1:4" x14ac:dyDescent="0.3">
@@ -15006,13 +15017,13 @@
         <v>4</v>
       </c>
       <c r="B1039" s="1">
-        <v>43250</v>
+        <v>44347</v>
       </c>
       <c r="C1039">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D1039">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1040" spans="1:4" x14ac:dyDescent="0.3">
@@ -15020,13 +15031,13 @@
         <v>4</v>
       </c>
       <c r="B1040" s="1">
-        <v>43251</v>
+        <v>44348</v>
       </c>
       <c r="C1040">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D1040">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1041" spans="1:4" x14ac:dyDescent="0.3">
@@ -15034,13 +15045,13 @@
         <v>4</v>
       </c>
       <c r="B1041" s="1">
-        <v>43252</v>
+        <v>44349</v>
       </c>
       <c r="C1041">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D1041">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1042" spans="1:4" x14ac:dyDescent="0.3">
@@ -15048,13 +15059,13 @@
         <v>4</v>
       </c>
       <c r="B1042" s="1">
-        <v>43253</v>
+        <v>44350</v>
       </c>
       <c r="C1042">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D1042">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1043" spans="1:4" x14ac:dyDescent="0.3">
@@ -15062,13 +15073,13 @@
         <v>4</v>
       </c>
       <c r="B1043" s="1">
-        <v>43254</v>
+        <v>44351</v>
       </c>
       <c r="C1043">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D1043">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1044" spans="1:4" x14ac:dyDescent="0.3">
@@ -15076,13 +15087,13 @@
         <v>4</v>
       </c>
       <c r="B1044" s="1">
-        <v>43255</v>
+        <v>44352</v>
       </c>
       <c r="C1044">
         <v>7</v>
       </c>
       <c r="D1044">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1045" spans="1:4" x14ac:dyDescent="0.3">
@@ -15090,13 +15101,13 @@
         <v>4</v>
       </c>
       <c r="B1045" s="1">
-        <v>43256</v>
+        <v>44353</v>
       </c>
       <c r="C1045">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1045">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1046" spans="1:4" x14ac:dyDescent="0.3">
@@ -15104,211 +15115,206 @@
         <v>4</v>
       </c>
       <c r="B1046" s="1">
-        <v>43257</v>
+        <v>44354</v>
       </c>
       <c r="C1046">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1046">
-        <v>2018</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1047" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1047" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1047" s="1">
-        <v>43258</v>
+        <v>44669</v>
       </c>
       <c r="C1047">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D1047">
-        <v>2018</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1048" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1048" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1048" s="1">
-        <v>44328</v>
+        <v>44670</v>
       </c>
       <c r="C1048">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1048">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1049" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1049" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1049" s="1">
-        <v>44329</v>
+        <v>44671</v>
       </c>
       <c r="C1049">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1049">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1050" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1050" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1050" s="1">
-        <v>44330</v>
+        <v>44672</v>
       </c>
       <c r="C1050">
-        <f>C1049-1/4</f>
-        <v>99.75</v>
+        <v>99</v>
       </c>
       <c r="D1050">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1051" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1051" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1051" s="1">
-        <v>44331</v>
+        <v>44673</v>
       </c>
       <c r="C1051">
-        <f t="shared" ref="C1051:C1052" si="13">C1050-1/4</f>
-        <v>99.5</v>
+        <v>97</v>
       </c>
       <c r="D1051">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1052" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1052" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1052" s="1">
-        <v>44332</v>
+        <v>44674</v>
       </c>
       <c r="C1052">
-        <f t="shared" si="13"/>
-        <v>99.25</v>
+        <v>90</v>
       </c>
       <c r="D1052">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1053" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1053" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1053" s="1">
-        <v>44333</v>
+        <v>44675</v>
       </c>
       <c r="C1053">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="D1053">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1054" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1054" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1054" s="1">
-        <v>44334</v>
+        <v>44676</v>
       </c>
       <c r="C1054">
-        <f>C1053-2/3</f>
-        <v>98.333333333333329</v>
+        <v>40</v>
       </c>
       <c r="D1054">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1055" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1055" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1055" s="1">
-        <v>44335</v>
+        <v>44677</v>
       </c>
       <c r="C1055">
-        <f>C1054-2/3</f>
-        <v>97.666666666666657</v>
+        <v>100</v>
       </c>
       <c r="D1055">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1056" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1056" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1056" s="1">
-        <v>44336</v>
+        <v>44679</v>
       </c>
       <c r="C1056">
-        <v>97</v>
+        <v>15</v>
       </c>
       <c r="D1056">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1057" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1057" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1057" s="1">
-        <v>44337</v>
+        <v>44680</v>
       </c>
       <c r="C1057">
-        <v>96</v>
+        <v>8</v>
       </c>
       <c r="D1057">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1058" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1058" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1058" s="1">
-        <v>44338</v>
+        <v>44681</v>
       </c>
       <c r="C1058">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D1058">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1059" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1059" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1059" s="1">
-        <v>44339</v>
+        <v>44682</v>
       </c>
       <c r="C1059">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="D1059">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="1060" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1060" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1060" s="1">
-        <v>44340</v>
+        <v>44266</v>
       </c>
       <c r="C1060">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D1060">
         <v>2021</v>
@@ -15316,13 +15322,13 @@
     </row>
     <row r="1061" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1061" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1061" s="1">
-        <v>44341</v>
+        <v>44267</v>
       </c>
       <c r="C1061">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D1061">
         <v>2021</v>
@@ -15330,13 +15336,13 @@
     </row>
     <row r="1062" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1062" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1062" s="1">
-        <v>44342</v>
+        <v>44268</v>
       </c>
       <c r="C1062">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D1062">
         <v>2021</v>
@@ -15344,14 +15350,13 @@
     </row>
     <row r="1063" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1063" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1063" s="1">
-        <v>44343</v>
+        <v>44269</v>
       </c>
       <c r="C1063">
-        <f>C1062-11/2</f>
-        <v>85.5</v>
+        <v>98</v>
       </c>
       <c r="D1063">
         <v>2021</v>
@@ -15359,13 +15364,13 @@
     </row>
     <row r="1064" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1064" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1064" s="1">
-        <v>44344</v>
+        <v>44270</v>
       </c>
       <c r="C1064">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="D1064">
         <v>2021</v>
@@ -15373,14 +15378,13 @@
     </row>
     <row r="1065" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1065" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1065" s="1">
-        <v>44345</v>
+        <v>44271</v>
       </c>
       <c r="C1065">
-        <f>C1064-24/3</f>
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D1065">
         <v>2021</v>
@@ -15388,14 +15392,13 @@
     </row>
     <row r="1066" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1066" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1066" s="1">
-        <v>44346</v>
+        <v>44272</v>
       </c>
       <c r="C1066">
-        <f>C1065-24/3</f>
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="D1066">
         <v>2021</v>
@@ -15403,13 +15406,13 @@
     </row>
     <row r="1067" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1067" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1067" s="1">
-        <v>44347</v>
+        <v>44273</v>
       </c>
       <c r="C1067">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="D1067">
         <v>2021</v>
@@ -15417,13 +15420,13 @@
     </row>
     <row r="1068" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1068" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1068" s="1">
-        <v>44348</v>
+        <v>44274</v>
       </c>
       <c r="C1068">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="D1068">
         <v>2021</v>
@@ -15431,13 +15434,13 @@
     </row>
     <row r="1069" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1069" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1069" s="1">
-        <v>44349</v>
+        <v>44275</v>
       </c>
       <c r="C1069">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="D1069">
         <v>2021</v>
@@ -15445,13 +15448,13 @@
     </row>
     <row r="1070" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1070" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1070" s="1">
-        <v>44350</v>
+        <v>44276</v>
       </c>
       <c r="C1070">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="D1070">
         <v>2021</v>
@@ -15459,13 +15462,13 @@
     </row>
     <row r="1071" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1071" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1071" s="1">
-        <v>44351</v>
+        <v>44277</v>
       </c>
       <c r="C1071">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="D1071">
         <v>2021</v>
@@ -15473,13 +15476,13 @@
     </row>
     <row r="1072" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1072" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1072" s="1">
-        <v>44352</v>
+        <v>44278</v>
       </c>
       <c r="C1072">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D1072">
         <v>2021</v>
@@ -15487,13 +15490,13 @@
     </row>
     <row r="1073" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1073" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1073" s="1">
-        <v>44353</v>
+        <v>44279</v>
       </c>
       <c r="C1073">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1073">
         <v>2021</v>
@@ -15501,13 +15504,13 @@
     </row>
     <row r="1074" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1074" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B1074" s="1">
-        <v>44354</v>
+        <v>44281</v>
       </c>
       <c r="C1074">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D1074">
         <v>2021</v>
@@ -15518,13 +15521,13 @@
         <v>11</v>
       </c>
       <c r="B1075" s="1">
-        <v>44669</v>
+        <v>44282</v>
       </c>
       <c r="C1075">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D1075">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1076" spans="1:4" x14ac:dyDescent="0.3">
@@ -15532,13 +15535,13 @@
         <v>11</v>
       </c>
       <c r="B1076" s="1">
-        <v>44670</v>
+        <v>44283</v>
       </c>
       <c r="C1076">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D1076">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1077" spans="1:4" x14ac:dyDescent="0.3">
@@ -15546,13 +15549,13 @@
         <v>11</v>
       </c>
       <c r="B1077" s="1">
-        <v>44671</v>
+        <v>44284</v>
       </c>
       <c r="C1077">
-        <v>99</v>
+        <v>30</v>
       </c>
       <c r="D1077">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1078" spans="1:4" x14ac:dyDescent="0.3">
@@ -15560,13 +15563,13 @@
         <v>11</v>
       </c>
       <c r="B1078" s="1">
-        <v>44672</v>
+        <v>44285</v>
       </c>
       <c r="C1078">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="D1078">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1079" spans="1:4" x14ac:dyDescent="0.3">
@@ -15574,13 +15577,13 @@
         <v>11</v>
       </c>
       <c r="B1079" s="1">
-        <v>44673</v>
+        <v>44287</v>
       </c>
       <c r="C1079">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="D1079">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1080" spans="1:4" x14ac:dyDescent="0.3">
@@ -15588,13 +15591,13 @@
         <v>11</v>
       </c>
       <c r="B1080" s="1">
-        <v>44674</v>
+        <v>44288</v>
       </c>
       <c r="C1080">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="D1080">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1081" spans="1:4" x14ac:dyDescent="0.3">
@@ -15602,13 +15605,13 @@
         <v>11</v>
       </c>
       <c r="B1081" s="1">
-        <v>44675</v>
+        <v>44289</v>
       </c>
       <c r="C1081">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="D1081">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1082" spans="1:4" x14ac:dyDescent="0.3">
@@ -15616,13 +15619,13 @@
         <v>11</v>
       </c>
       <c r="B1082" s="1">
-        <v>44676</v>
+        <v>44290</v>
       </c>
       <c r="C1082">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D1082">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1083" spans="1:4" x14ac:dyDescent="0.3">
@@ -15630,13 +15633,13 @@
         <v>11</v>
       </c>
       <c r="B1083" s="1">
-        <v>44677</v>
+        <v>44291</v>
       </c>
       <c r="C1083">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D1083">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1084" spans="1:4" x14ac:dyDescent="0.3">
@@ -15644,13 +15647,13 @@
         <v>11</v>
       </c>
       <c r="B1084" s="1">
-        <v>44679</v>
+        <v>44292</v>
       </c>
       <c r="C1084">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D1084">
-        <v>2022</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="1085" spans="1:4" x14ac:dyDescent="0.3">
@@ -15658,13 +15661,13 @@
         <v>11</v>
       </c>
       <c r="B1085" s="1">
-        <v>44680</v>
+        <v>43916</v>
       </c>
       <c r="C1085">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="D1085">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="1086" spans="1:4" x14ac:dyDescent="0.3">
@@ -15672,13 +15675,13 @@
         <v>11</v>
       </c>
       <c r="B1086" s="1">
-        <v>44681</v>
+        <v>43917</v>
       </c>
       <c r="C1086">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="D1086">
-        <v>2022</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="1087" spans="1:4" x14ac:dyDescent="0.3">
@@ -15686,13 +15689,1637 @@
         <v>11</v>
       </c>
       <c r="B1087" s="1">
-        <v>44682</v>
+        <v>43918</v>
       </c>
       <c r="C1087">
+        <v>99</v>
+      </c>
+      <c r="D1087">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1088" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1088" s="1">
+        <v>43919</v>
+      </c>
+      <c r="C1088">
+        <v>98</v>
+      </c>
+      <c r="D1088">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1089" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1089" s="1">
+        <v>43920</v>
+      </c>
+      <c r="C1089">
+        <v>97</v>
+      </c>
+      <c r="D1089">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1090" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1090" s="1">
+        <v>43921</v>
+      </c>
+      <c r="C1090">
+        <v>96</v>
+      </c>
+      <c r="D1090">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1091" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1091" s="1">
+        <v>43922</v>
+      </c>
+      <c r="C1091">
+        <v>95</v>
+      </c>
+      <c r="D1091">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1092" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1092" s="1">
+        <v>43923</v>
+      </c>
+      <c r="C1092">
+        <v>92</v>
+      </c>
+      <c r="D1092">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1093" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1093" s="1">
+        <v>43924</v>
+      </c>
+      <c r="C1093">
+        <v>85</v>
+      </c>
+      <c r="D1093">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1094" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1094" s="1">
+        <v>43925</v>
+      </c>
+      <c r="C1094">
+        <v>84</v>
+      </c>
+      <c r="D1094">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1095" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1095" s="1">
+        <v>43926</v>
+      </c>
+      <c r="C1095">
+        <v>80</v>
+      </c>
+      <c r="D1095">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1096" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1096" s="1">
+        <v>43927</v>
+      </c>
+      <c r="C1096">
+        <v>75</v>
+      </c>
+      <c r="D1096">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1097" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1097" s="1">
+        <v>43928</v>
+      </c>
+      <c r="C1097">
+        <v>70</v>
+      </c>
+      <c r="D1097">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1098" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1098" s="1">
+        <v>43929</v>
+      </c>
+      <c r="C1098">
+        <v>50</v>
+      </c>
+      <c r="D1098">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1099" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1099" s="1">
+        <v>43930</v>
+      </c>
+      <c r="C1099">
+        <v>40</v>
+      </c>
+      <c r="D1099">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1100" s="1">
+        <v>43931</v>
+      </c>
+      <c r="C1100">
+        <v>40</v>
+      </c>
+      <c r="D1100">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1101" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1101" s="1">
+        <v>43932</v>
+      </c>
+      <c r="C1101">
+        <v>25</v>
+      </c>
+      <c r="D1101">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1102" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1102" s="1">
+        <v>43933</v>
+      </c>
+      <c r="C1102">
+        <v>100</v>
+      </c>
+      <c r="D1102">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1103" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1103" s="1">
+        <v>43934</v>
+      </c>
+      <c r="C1103">
+        <v>100</v>
+      </c>
+      <c r="D1103">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1104" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1104" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C1104">
+        <v>100</v>
+      </c>
+      <c r="D1104">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1105" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1105" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C1105">
+        <v>100</v>
+      </c>
+      <c r="D1105">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1106" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1106" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C1106">
+        <v>100</v>
+      </c>
+      <c r="D1106">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1107" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1107" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C1107">
+        <v>97</v>
+      </c>
+      <c r="D1107">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1108" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1108" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C1108">
+        <v>50</v>
+      </c>
+      <c r="D1108">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1109" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1109" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C1109">
+        <v>15</v>
+      </c>
+      <c r="D1109">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1110" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1110" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C1110">
+        <v>15</v>
+      </c>
+      <c r="D1110">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1111" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1111" s="1">
+        <v>43942</v>
+      </c>
+      <c r="C1111">
+        <v>15</v>
+      </c>
+      <c r="D1111">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1112" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1112" s="1">
+        <v>43943</v>
+      </c>
+      <c r="C1112">
+        <v>15</v>
+      </c>
+      <c r="D1112">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1113" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1113" s="1">
+        <v>43944</v>
+      </c>
+      <c r="C1113">
+        <v>10</v>
+      </c>
+      <c r="D1113">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1114" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1114" s="1">
+        <v>43945</v>
+      </c>
+      <c r="C1114">
+        <v>6</v>
+      </c>
+      <c r="D1114">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1115" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1115" s="1">
+        <v>43946</v>
+      </c>
+      <c r="C1115">
+        <v>3</v>
+      </c>
+      <c r="D1115">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1116" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1116" s="1">
+        <v>43947</v>
+      </c>
+      <c r="C1116">
+        <v>2</v>
+      </c>
+      <c r="D1116">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1117" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1117" s="1">
+        <v>43948</v>
+      </c>
+      <c r="C1117">
+        <v>1</v>
+      </c>
+      <c r="D1117">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1118" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1118" s="1">
+        <v>43949</v>
+      </c>
+      <c r="C1118">
+        <v>1</v>
+      </c>
+      <c r="D1118">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1119" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1119" s="1">
+        <v>43950</v>
+      </c>
+      <c r="C1119">
         <v>0</v>
       </c>
-      <c r="D1087">
-        <v>2022</v>
+      <c r="D1119">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1120" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1120" s="1">
+        <v>43561</v>
+      </c>
+      <c r="C1120">
+        <v>100</v>
+      </c>
+      <c r="D1120">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1121" s="1">
+        <v>43562</v>
+      </c>
+      <c r="C1121">
+        <v>99</v>
+      </c>
+      <c r="D1121">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1122" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1122" s="1">
+        <v>43563</v>
+      </c>
+      <c r="C1122">
+        <v>97</v>
+      </c>
+      <c r="D1122">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1123" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1123" s="1">
+        <v>43564</v>
+      </c>
+      <c r="C1123">
+        <v>96</v>
+      </c>
+      <c r="D1123">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1124" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1124" s="1">
+        <v>43565</v>
+      </c>
+      <c r="C1124">
+        <v>95</v>
+      </c>
+      <c r="D1124">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1125" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1125" s="1">
+        <v>43566</v>
+      </c>
+      <c r="C1125">
+        <v>100</v>
+      </c>
+      <c r="D1125">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1126" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1126" s="1">
+        <v>43567</v>
+      </c>
+      <c r="C1126">
+        <v>100</v>
+      </c>
+      <c r="D1126">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1127" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1127" s="1">
+        <v>43568</v>
+      </c>
+      <c r="C1127">
+        <v>100</v>
+      </c>
+      <c r="D1127">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1128" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1128" s="1">
+        <v>43569</v>
+      </c>
+      <c r="C1128">
+        <v>100</v>
+      </c>
+      <c r="D1128">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1129" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1129" s="1">
+        <v>43570</v>
+      </c>
+      <c r="C1129">
+        <v>100</v>
+      </c>
+      <c r="D1129">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1130" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1130" s="1">
+        <v>43571</v>
+      </c>
+      <c r="C1130">
+        <v>95</v>
+      </c>
+      <c r="D1130">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1131" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1131" s="1">
+        <v>43572</v>
+      </c>
+      <c r="C1131">
+        <v>87</v>
+      </c>
+      <c r="D1131">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1132" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1132" s="1">
+        <v>43573</v>
+      </c>
+      <c r="C1132">
+        <v>85</v>
+      </c>
+      <c r="D1132">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1133" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1133" s="1">
+        <v>43574</v>
+      </c>
+      <c r="C1133">
+        <v>75</v>
+      </c>
+      <c r="D1133">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1134" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1134" s="1">
+        <v>43575</v>
+      </c>
+      <c r="C1134">
+        <v>60</v>
+      </c>
+      <c r="D1134">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1135" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1135" s="1">
+        <v>43576</v>
+      </c>
+      <c r="C1135">
+        <v>30</v>
+      </c>
+      <c r="D1135">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1136" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1136" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C1136">
+        <v>25</v>
+      </c>
+      <c r="D1136">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1137" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1137" s="1">
+        <v>43578</v>
+      </c>
+      <c r="C1137">
+        <v>10</v>
+      </c>
+      <c r="D1137">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1138" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1138" s="1">
+        <v>43579</v>
+      </c>
+      <c r="C1138">
+        <v>5</v>
+      </c>
+      <c r="D1138">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1139" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1139" s="1">
+        <v>43580</v>
+      </c>
+      <c r="C1139">
+        <v>3</v>
+      </c>
+      <c r="D1139">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1140" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1140" s="1">
+        <v>43581</v>
+      </c>
+      <c r="C1140">
+        <v>2</v>
+      </c>
+      <c r="D1140">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1141" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1141" s="1">
+        <v>43582</v>
+      </c>
+      <c r="C1141">
+        <v>1</v>
+      </c>
+      <c r="D1141">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1142" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1142" s="1">
+        <v>43583</v>
+      </c>
+      <c r="C1142">
+        <v>1</v>
+      </c>
+      <c r="D1142">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1143" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1143" s="1">
+        <v>43584</v>
+      </c>
+      <c r="C1143">
+        <v>1</v>
+      </c>
+      <c r="D1143">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1144" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1144" s="1">
+        <v>43585</v>
+      </c>
+      <c r="C1144">
+        <v>0</v>
+      </c>
+      <c r="D1144">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1145" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1145" s="1">
+        <v>44636</v>
+      </c>
+      <c r="C1145">
+        <v>100</v>
+      </c>
+      <c r="D1145">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1146" s="1">
+        <v>44637</v>
+      </c>
+      <c r="C1146">
+        <v>99</v>
+      </c>
+      <c r="D1146">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1147" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1147" s="1">
+        <v>44638</v>
+      </c>
+      <c r="C1147">
+        <v>98</v>
+      </c>
+      <c r="D1147">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1148" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1148" s="1">
+        <v>44639</v>
+      </c>
+      <c r="C1148">
+        <v>97</v>
+      </c>
+      <c r="D1148">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1149" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1149" s="1">
+        <v>44640</v>
+      </c>
+      <c r="C1149">
+        <v>95</v>
+      </c>
+      <c r="D1149">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1150" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1150" s="1">
+        <v>44641</v>
+      </c>
+      <c r="C1150">
+        <v>90</v>
+      </c>
+      <c r="D1150">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1151" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1151" s="1">
+        <v>44642</v>
+      </c>
+      <c r="C1151">
+        <v>85</v>
+      </c>
+      <c r="D1151">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1152" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1152" s="1">
+        <v>44643</v>
+      </c>
+      <c r="C1152">
+        <v>80</v>
+      </c>
+      <c r="D1152">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1153" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1153" s="1">
+        <v>44644</v>
+      </c>
+      <c r="C1153">
+        <v>100</v>
+      </c>
+      <c r="D1153">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1154" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1154" s="1">
+        <v>44645</v>
+      </c>
+      <c r="C1154">
+        <v>70</v>
+      </c>
+      <c r="D1154">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1155" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1155" s="1">
+        <v>44646</v>
+      </c>
+      <c r="C1155">
+        <v>55</v>
+      </c>
+      <c r="D1155">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1156" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1156" s="1">
+        <v>44647</v>
+      </c>
+      <c r="C1156">
+        <v>45</v>
+      </c>
+      <c r="D1156">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1157" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1157" s="1">
+        <v>44648</v>
+      </c>
+      <c r="C1157">
+        <v>40</v>
+      </c>
+      <c r="D1157">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1158" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1158" s="1">
+        <v>44649</v>
+      </c>
+      <c r="C1158">
+        <v>40</v>
+      </c>
+      <c r="D1158">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1159" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1159" s="1">
+        <v>44650</v>
+      </c>
+      <c r="C1159">
+        <v>35</v>
+      </c>
+      <c r="D1159">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1160" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1160" s="1">
+        <v>44651</v>
+      </c>
+      <c r="C1160">
+        <v>20</v>
+      </c>
+      <c r="D1160">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1161" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1161" s="1">
+        <v>44652</v>
+      </c>
+      <c r="C1161">
+        <v>10</v>
+      </c>
+      <c r="D1161">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1162" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1162" s="1">
+        <v>44653</v>
+      </c>
+      <c r="C1162">
+        <v>5</v>
+      </c>
+      <c r="D1162">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1163" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1163" s="1">
+        <v>44654</v>
+      </c>
+      <c r="C1163">
+        <v>4</v>
+      </c>
+      <c r="D1163">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1164" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1164" s="1">
+        <v>44655</v>
+      </c>
+      <c r="C1164">
+        <v>2</v>
+      </c>
+      <c r="D1164">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1165" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1165" s="1">
+        <v>44656</v>
+      </c>
+      <c r="C1165">
+        <v>1</v>
+      </c>
+      <c r="D1165">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1166" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1166" s="1">
+        <v>44657</v>
+      </c>
+      <c r="C1166">
+        <v>0</v>
+      </c>
+      <c r="D1166">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1167" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1167" s="1">
+        <v>44279</v>
+      </c>
+      <c r="C1167">
+        <v>98</v>
+      </c>
+      <c r="D1167">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1168" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1168" s="1">
+        <v>44280</v>
+      </c>
+      <c r="C1168">
+        <v>96</v>
+      </c>
+      <c r="D1168">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1169" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1169" s="1">
+        <v>44281</v>
+      </c>
+      <c r="C1169">
+        <v>94</v>
+      </c>
+      <c r="D1169">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1170" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1170" s="1">
+        <v>44282</v>
+      </c>
+      <c r="C1170">
+        <v>87</v>
+      </c>
+      <c r="D1170">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1171" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1171" s="1">
+        <v>44283</v>
+      </c>
+      <c r="C1171">
+        <v>85</v>
+      </c>
+      <c r="D1171">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1172" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1172" s="1">
+        <v>44284</v>
+      </c>
+      <c r="C1172">
+        <v>75</v>
+      </c>
+      <c r="D1172">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1173" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1173" s="1">
+        <v>44285</v>
+      </c>
+      <c r="C1173">
+        <v>65</v>
+      </c>
+      <c r="D1173">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1174" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1174" s="1">
+        <v>44286</v>
+      </c>
+      <c r="C1174">
+        <v>40</v>
+      </c>
+      <c r="D1174">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1175" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1175" s="1">
+        <v>44287</v>
+      </c>
+      <c r="C1175">
+        <v>20</v>
+      </c>
+      <c r="D1175">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1176" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1176" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C1176">
+        <v>15</v>
+      </c>
+      <c r="D1176">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1177" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1177" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C1177">
+        <v>10</v>
+      </c>
+      <c r="D1177">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1178" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1178" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C1178">
+        <v>5</v>
+      </c>
+      <c r="D1178">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1179" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1179" s="1">
+        <v>44291</v>
+      </c>
+      <c r="C1179">
+        <v>2</v>
+      </c>
+      <c r="D1179">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1180" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1180" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C1180">
+        <v>0</v>
+      </c>
+      <c r="D1180">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1181" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1181" s="1">
+        <v>43926</v>
+      </c>
+      <c r="C1181">
+        <v>95</v>
+      </c>
+      <c r="D1181">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1182" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1182" s="1">
+        <v>43927</v>
+      </c>
+      <c r="C1182">
+        <v>90</v>
+      </c>
+      <c r="D1182">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1183" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1183" s="1">
+        <v>43928</v>
+      </c>
+      <c r="C1183">
+        <v>87</v>
+      </c>
+      <c r="D1183">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1184" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1184" s="1">
+        <v>43929</v>
+      </c>
+      <c r="C1184">
+        <v>85</v>
+      </c>
+      <c r="D1184">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1185" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1185" s="1">
+        <v>43934</v>
+      </c>
+      <c r="C1185">
+        <v>78</v>
+      </c>
+      <c r="D1185">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1186" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1186" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C1186">
+        <v>45</v>
+      </c>
+      <c r="D1186">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1187" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1187" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C1187">
+        <v>40</v>
+      </c>
+      <c r="D1187">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1188" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1188" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C1188">
+        <v>35</v>
+      </c>
+      <c r="D1188">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1189" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1189" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C1189">
+        <v>30</v>
+      </c>
+      <c r="D1189">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1190" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1190" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C1190">
+        <v>25</v>
+      </c>
+      <c r="D1190">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1191" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1191" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C1191">
+        <v>15</v>
+      </c>
+      <c r="D1191">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1192" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1192" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C1192">
+        <v>5</v>
+      </c>
+      <c r="D1192">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1193" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1193" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C1193">
+        <v>95</v>
+      </c>
+      <c r="D1193">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1194" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1194" s="1">
+        <v>43578</v>
+      </c>
+      <c r="C1194">
+        <v>85</v>
+      </c>
+      <c r="D1194">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1195" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1195" s="1">
+        <v>43579</v>
+      </c>
+      <c r="C1195">
+        <v>75</v>
+      </c>
+      <c r="D1195">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1196" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1196" s="1">
+        <v>43580</v>
+      </c>
+      <c r="C1196">
+        <v>60</v>
+      </c>
+      <c r="D1196">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1197" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1197" s="1">
+        <v>43581</v>
+      </c>
+      <c r="C1197">
+        <v>60</v>
+      </c>
+      <c r="D1197">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1198" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1198" s="1">
+        <v>43582</v>
+      </c>
+      <c r="C1198">
+        <v>45</v>
+      </c>
+      <c r="D1198">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1199" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1199" s="1">
+        <v>43583</v>
+      </c>
+      <c r="C1199">
+        <v>20</v>
+      </c>
+      <c r="D1199">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1200" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1200" s="1">
+        <v>43584</v>
+      </c>
+      <c r="C1200">
+        <v>12</v>
+      </c>
+      <c r="D1200">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1201" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1201" s="1">
+        <v>43585</v>
+      </c>
+      <c r="C1201">
+        <v>5</v>
+      </c>
+      <c r="D1201">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1202" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1202" s="1">
+        <v>43586</v>
+      </c>
+      <c r="C1202">
+        <v>2</v>
+      </c>
+      <c r="D1202">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1203" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1203" s="1">
+        <v>43587</v>
+      </c>
+      <c r="C1203">
+        <v>1</v>
+      </c>
+      <c r="D1203">
+        <v>2019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated FSC classifications, US sites done
</commit_message>
<xml_diff>
--- a/snow_timeline.xlsx
+++ b/snow_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1705EC-1B27-4D1B-AFE7-24D28A843343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E205646-126C-4412-941F-01FB9E3351D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5868" yWindow="372" windowWidth="17280" windowHeight="9960" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="16">
   <si>
     <t>Location</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>bartlett</t>
+  </si>
+  <si>
+    <t>underhill</t>
+  </si>
+  <si>
+    <t>willowcreek</t>
+  </si>
+  <si>
+    <t>glees</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0BDC52-0678-4879-BFA4-045E88D6C76C}">
-  <dimension ref="A1:D1203"/>
+  <dimension ref="A1:D1278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1177" workbookViewId="0">
-      <selection activeCell="D1193" sqref="D1193:D1203"/>
+    <sheetView tabSelected="1" topLeftCell="A1259" workbookViewId="0">
+      <selection activeCell="J1278" sqref="J1278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17322,6 +17331,1056 @@
         <v>2019</v>
       </c>
     </row>
+    <row r="1204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1204" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1204" s="1">
+        <v>44626</v>
+      </c>
+      <c r="C1204">
+        <v>98</v>
+      </c>
+      <c r="D1204">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1205" s="1">
+        <v>44627</v>
+      </c>
+      <c r="C1205">
+        <v>7</v>
+      </c>
+      <c r="D1205">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1206" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1206" s="1">
+        <v>44628</v>
+      </c>
+      <c r="C1206">
+        <v>15</v>
+      </c>
+      <c r="D1206">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1207" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1207" s="1">
+        <v>44629</v>
+      </c>
+      <c r="C1207">
+        <v>7</v>
+      </c>
+      <c r="D1207">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1208" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1208" s="1">
+        <v>44630</v>
+      </c>
+      <c r="C1208">
+        <v>7</v>
+      </c>
+      <c r="D1208">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1209" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1209" s="1">
+        <v>44631</v>
+      </c>
+      <c r="C1209">
+        <v>5</v>
+      </c>
+      <c r="D1209">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1210" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1210" s="1">
+        <v>44636</v>
+      </c>
+      <c r="C1210">
+        <v>100</v>
+      </c>
+      <c r="D1210">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1211" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1211" s="1">
+        <v>44637</v>
+      </c>
+      <c r="C1211">
+        <v>3</v>
+      </c>
+      <c r="D1211">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1212" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1212" s="1">
+        <v>44638</v>
+      </c>
+      <c r="C1212">
+        <v>1</v>
+      </c>
+      <c r="D1212">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1213" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1213" s="1">
+        <v>44267</v>
+      </c>
+      <c r="C1213">
+        <v>95</v>
+      </c>
+      <c r="D1213">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1214" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1214" s="1">
+        <v>44268</v>
+      </c>
+      <c r="C1214">
+        <v>90</v>
+      </c>
+      <c r="D1214">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1215" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1215" s="1">
+        <v>44270</v>
+      </c>
+      <c r="C1215">
+        <v>100</v>
+      </c>
+      <c r="D1215">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1216" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1216" s="1">
+        <v>44271</v>
+      </c>
+      <c r="C1216">
+        <v>98</v>
+      </c>
+      <c r="D1216">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1217" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1217" s="1">
+        <v>44272</v>
+      </c>
+      <c r="C1217">
+        <v>85</v>
+      </c>
+      <c r="D1217">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1218" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1218" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C1218">
+        <v>80</v>
+      </c>
+      <c r="D1218">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1219" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1219" s="1">
+        <v>44274</v>
+      </c>
+      <c r="C1219">
+        <v>80</v>
+      </c>
+      <c r="D1219">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1220" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1220" s="1">
+        <v>44275</v>
+      </c>
+      <c r="C1220">
+        <v>75</v>
+      </c>
+      <c r="D1220">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1221" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1221" s="1">
+        <v>44276</v>
+      </c>
+      <c r="C1221">
+        <v>65</v>
+      </c>
+      <c r="D1221">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1222" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1222" s="1">
+        <v>43898</v>
+      </c>
+      <c r="C1222">
+        <v>97</v>
+      </c>
+      <c r="D1222">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1223" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1223" s="1">
+        <v>43899</v>
+      </c>
+      <c r="C1223">
+        <v>90</v>
+      </c>
+      <c r="D1223">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1224" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1224" s="1">
+        <v>43900</v>
+      </c>
+      <c r="C1224">
+        <v>60</v>
+      </c>
+      <c r="D1224">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1225" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1225" s="1">
+        <v>43901</v>
+      </c>
+      <c r="C1225">
+        <v>25</v>
+      </c>
+      <c r="D1225">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1226" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1226" s="1">
+        <v>43902</v>
+      </c>
+      <c r="C1226">
+        <v>25</v>
+      </c>
+      <c r="D1226">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1227" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1227" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C1227">
+        <v>10</v>
+      </c>
+      <c r="D1227">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1228" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1228" s="1">
+        <v>43904</v>
+      </c>
+      <c r="C1228">
+        <v>5</v>
+      </c>
+      <c r="D1228">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1229" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1229" s="1">
+        <v>43539</v>
+      </c>
+      <c r="C1229">
+        <v>90</v>
+      </c>
+      <c r="D1229">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1230" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1230" s="1">
+        <v>43540</v>
+      </c>
+      <c r="C1230">
+        <v>90</v>
+      </c>
+      <c r="D1230">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1231" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1231" s="1">
+        <v>43542</v>
+      </c>
+      <c r="C1231">
+        <v>90</v>
+      </c>
+      <c r="D1231">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1232" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1232" s="1">
+        <v>43544</v>
+      </c>
+      <c r="C1232">
+        <v>80</v>
+      </c>
+      <c r="D1232">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1233" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1233" s="1">
+        <v>43545</v>
+      </c>
+      <c r="C1233">
+        <v>65</v>
+      </c>
+      <c r="D1233">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1234" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1234" s="1">
+        <v>43553</v>
+      </c>
+      <c r="C1234">
+        <v>95</v>
+      </c>
+      <c r="D1234">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1235" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1235" s="1">
+        <v>43555</v>
+      </c>
+      <c r="C1235">
+        <v>5</v>
+      </c>
+      <c r="D1235">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1236" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1236" s="1">
+        <v>43557</v>
+      </c>
+      <c r="C1236">
+        <v>5</v>
+      </c>
+      <c r="D1236">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1237" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1237" s="1">
+        <v>44663</v>
+      </c>
+      <c r="C1237">
+        <v>90</v>
+      </c>
+      <c r="D1237">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1238" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1238" s="1">
+        <v>44664</v>
+      </c>
+      <c r="C1238">
+        <v>75</v>
+      </c>
+      <c r="D1238">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1239" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1239" s="1">
+        <v>44668</v>
+      </c>
+      <c r="C1239">
+        <v>70</v>
+      </c>
+      <c r="D1239">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1240" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1240" s="1">
+        <v>44671</v>
+      </c>
+      <c r="C1240">
+        <v>40</v>
+      </c>
+      <c r="D1240">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1241" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1241" s="1">
+        <v>44672</v>
+      </c>
+      <c r="C1241">
+        <v>10</v>
+      </c>
+      <c r="D1241">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1242" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1242" s="1">
+        <v>44673</v>
+      </c>
+      <c r="C1242">
+        <v>2</v>
+      </c>
+      <c r="D1242">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1243" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1243" s="1">
+        <v>44272</v>
+      </c>
+      <c r="C1243">
+        <v>97</v>
+      </c>
+      <c r="D1243">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1244" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1244" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C1244">
+        <v>96</v>
+      </c>
+      <c r="D1244">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1245" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1245" s="1">
+        <v>44274</v>
+      </c>
+      <c r="C1245">
+        <v>95</v>
+      </c>
+      <c r="D1245">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1246" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1246" s="1">
+        <v>44275</v>
+      </c>
+      <c r="C1246">
+        <v>92</v>
+      </c>
+      <c r="D1246">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1247" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1247" s="1">
+        <v>44276</v>
+      </c>
+      <c r="C1247">
+        <v>80</v>
+      </c>
+      <c r="D1247">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1248" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1248" s="1">
+        <v>44277</v>
+      </c>
+      <c r="C1248">
+        <v>7</v>
+      </c>
+      <c r="D1248">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1249" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1249" s="1">
+        <v>43923</v>
+      </c>
+      <c r="C1249">
+        <v>90</v>
+      </c>
+      <c r="D1249">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1250" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1250" s="1">
+        <v>43924</v>
+      </c>
+      <c r="C1250">
+        <v>70</v>
+      </c>
+      <c r="D1250">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1251" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1251" s="1">
+        <v>43926</v>
+      </c>
+      <c r="C1251">
+        <v>50</v>
+      </c>
+      <c r="D1251">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1252" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1252" s="1">
+        <v>43927</v>
+      </c>
+      <c r="C1252">
+        <v>25</v>
+      </c>
+      <c r="D1252">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1253" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1253" s="1">
+        <v>43928</v>
+      </c>
+      <c r="C1253">
+        <v>5</v>
+      </c>
+      <c r="D1253">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1254" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1254" s="1">
+        <v>43574</v>
+      </c>
+      <c r="C1254">
+        <v>97</v>
+      </c>
+      <c r="D1254">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1255" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1255" s="1">
+        <v>43575</v>
+      </c>
+      <c r="C1255">
+        <v>85</v>
+      </c>
+      <c r="D1255">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1256" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1256" s="1">
+        <v>43576</v>
+      </c>
+      <c r="C1256">
+        <v>45</v>
+      </c>
+      <c r="D1256">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1257" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1257" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C1257">
+        <v>10</v>
+      </c>
+      <c r="D1257">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1258" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1258" s="1">
+        <v>44715</v>
+      </c>
+      <c r="C1258">
+        <v>95</v>
+      </c>
+      <c r="D1258">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1259" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1259" s="1">
+        <v>44716</v>
+      </c>
+      <c r="C1259">
+        <v>93</v>
+      </c>
+      <c r="D1259">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1260" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1260" s="1">
+        <v>44717</v>
+      </c>
+      <c r="C1260">
+        <v>89</v>
+      </c>
+      <c r="D1260">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1261" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1261" s="1">
+        <v>44718</v>
+      </c>
+      <c r="C1261">
+        <v>83</v>
+      </c>
+      <c r="D1261">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1262" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1262" s="1">
+        <v>44719</v>
+      </c>
+      <c r="C1262">
+        <v>75</v>
+      </c>
+      <c r="D1262">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1263" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1263" s="1">
+        <v>44720</v>
+      </c>
+      <c r="C1263">
+        <v>70</v>
+      </c>
+      <c r="D1263">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1264" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1264" s="1">
+        <v>44721</v>
+      </c>
+      <c r="C1264">
+        <v>60</v>
+      </c>
+      <c r="D1264">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1265" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1265" s="1">
+        <v>44722</v>
+      </c>
+      <c r="C1265">
+        <v>45</v>
+      </c>
+      <c r="D1265">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1266" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1266" s="1">
+        <v>44723</v>
+      </c>
+      <c r="C1266">
+        <v>25</v>
+      </c>
+      <c r="D1266">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1267" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1267" s="1">
+        <v>44724</v>
+      </c>
+      <c r="C1267">
+        <v>15</v>
+      </c>
+      <c r="D1267">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1268" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1268" s="1">
+        <v>44725</v>
+      </c>
+      <c r="C1268">
+        <v>10</v>
+      </c>
+      <c r="D1268">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1269" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1269" s="1">
+        <v>44726</v>
+      </c>
+      <c r="C1269">
+        <v>7</v>
+      </c>
+      <c r="D1269">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1270" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1270" s="1">
+        <v>44727</v>
+      </c>
+      <c r="C1270">
+        <v>5</v>
+      </c>
+      <c r="D1270">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1271" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1271" s="1">
+        <v>44728</v>
+      </c>
+      <c r="C1271">
+        <v>3</v>
+      </c>
+      <c r="D1271">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1272" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1272" s="1">
+        <v>44350</v>
+      </c>
+      <c r="C1272">
+        <v>93</v>
+      </c>
+      <c r="D1272">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1273" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1273" s="1">
+        <v>44351</v>
+      </c>
+      <c r="C1273">
+        <v>85</v>
+      </c>
+      <c r="D1273">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1274" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1274" s="1">
+        <v>44352</v>
+      </c>
+      <c r="C1274">
+        <v>80</v>
+      </c>
+      <c r="D1274">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1275" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1275" s="1">
+        <v>44353</v>
+      </c>
+      <c r="C1275">
+        <v>70</v>
+      </c>
+      <c r="D1275">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1276" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1276" s="1">
+        <v>44354</v>
+      </c>
+      <c r="C1276">
+        <v>60</v>
+      </c>
+      <c r="D1276">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1277" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1277" s="1">
+        <v>44355</v>
+      </c>
+      <c r="C1277">
+        <v>45</v>
+      </c>
+      <c r="D1277">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1278" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1278" s="1">
+        <v>44356</v>
+      </c>
+      <c r="C1278">
+        <v>25</v>
+      </c>
+      <c r="D1278">
+        <v>2021</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated snow timeline, canada sites done
</commit_message>
<xml_diff>
--- a/snow_timeline.xlsx
+++ b/snow_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E205646-126C-4412-941F-01FB9E3351D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F89BA7-5D69-42BA-BAFE-879A18F8CDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
+    <workbookView xWindow="5868" yWindow="-12" windowWidth="17280" windowHeight="9960" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="18">
   <si>
     <t>Location</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>glees</t>
+  </si>
+  <si>
+    <t>queens</t>
+  </si>
+  <si>
+    <t>old_jack_pine</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0BDC52-0678-4879-BFA4-045E88D6C76C}">
-  <dimension ref="A1:D1278"/>
+  <dimension ref="A1:D1364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1259" workbookViewId="0">
-      <selection activeCell="J1278" sqref="J1278"/>
+    <sheetView tabSelected="1" topLeftCell="A1337" workbookViewId="0">
+      <selection activeCell="C1365" sqref="C1365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18381,6 +18387,1210 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="1279" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1279" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1279" s="1">
+        <v>44634</v>
+      </c>
+      <c r="C1279">
+        <v>98</v>
+      </c>
+      <c r="D1279">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1280" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1280" s="1">
+        <v>44635</v>
+      </c>
+      <c r="C1280">
+        <v>96</v>
+      </c>
+      <c r="D1280">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1281" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1281" s="1">
+        <v>44636</v>
+      </c>
+      <c r="C1281">
+        <v>95</v>
+      </c>
+      <c r="D1281">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1282" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1282" s="1">
+        <v>44637</v>
+      </c>
+      <c r="C1282">
+        <v>94</v>
+      </c>
+      <c r="D1282">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1283" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1283" s="1">
+        <v>44638</v>
+      </c>
+      <c r="C1283">
+        <v>93</v>
+      </c>
+      <c r="D1283">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1284" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1284" s="1">
+        <v>44639</v>
+      </c>
+      <c r="C1284">
+        <v>91</v>
+      </c>
+      <c r="D1284">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1285" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1285" s="1">
+        <v>44640</v>
+      </c>
+      <c r="C1285">
+        <v>90</v>
+      </c>
+      <c r="D1285">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1286" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1286" s="1">
+        <v>44641</v>
+      </c>
+      <c r="C1286">
+        <v>87</v>
+      </c>
+      <c r="D1286">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1287" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1287" s="1">
+        <v>44642</v>
+      </c>
+      <c r="C1287">
+        <v>83</v>
+      </c>
+      <c r="D1287">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1288" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1288" s="1">
+        <v>44643</v>
+      </c>
+      <c r="C1288">
+        <v>79</v>
+      </c>
+      <c r="D1288">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1289" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1289" s="1">
+        <v>44644</v>
+      </c>
+      <c r="C1289">
+        <v>50</v>
+      </c>
+      <c r="D1289">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1290" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1290" s="1">
+        <v>44645</v>
+      </c>
+      <c r="C1290">
+        <v>25</v>
+      </c>
+      <c r="D1290">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1291" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1291" s="1">
+        <v>44646</v>
+      </c>
+      <c r="C1291">
+        <v>12</v>
+      </c>
+      <c r="D1291">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1292" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1292" s="1">
+        <v>44647</v>
+      </c>
+      <c r="C1292">
+        <v>7</v>
+      </c>
+      <c r="D1292">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1293" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1293" s="1">
+        <v>44648</v>
+      </c>
+      <c r="C1293">
+        <v>6</v>
+      </c>
+      <c r="D1293">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1294" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1294" s="1">
+        <v>44649</v>
+      </c>
+      <c r="C1294">
+        <v>5</v>
+      </c>
+      <c r="D1294">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1295" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1295" s="1">
+        <v>44265</v>
+      </c>
+      <c r="C1295">
+        <v>97</v>
+      </c>
+      <c r="D1295">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1296" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1296" s="1">
+        <v>44266</v>
+      </c>
+      <c r="C1296">
+        <v>90</v>
+      </c>
+      <c r="D1296">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1297" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1297" s="1">
+        <v>44267</v>
+      </c>
+      <c r="C1297">
+        <v>75</v>
+      </c>
+      <c r="D1297">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1298" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1298" s="1">
+        <v>44268</v>
+      </c>
+      <c r="C1298">
+        <v>45</v>
+      </c>
+      <c r="D1298">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1299" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1299" s="1">
+        <v>44269</v>
+      </c>
+      <c r="C1299">
+        <v>40</v>
+      </c>
+      <c r="D1299">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1300" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1300" s="1">
+        <v>44270</v>
+      </c>
+      <c r="C1300">
+        <v>38</v>
+      </c>
+      <c r="D1300">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1301" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1301" s="1">
+        <v>44271</v>
+      </c>
+      <c r="C1301">
+        <v>37</v>
+      </c>
+      <c r="D1301">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1302" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1302" s="1">
+        <v>44272</v>
+      </c>
+      <c r="C1302">
+        <v>25</v>
+      </c>
+      <c r="D1302">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1303" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1303" s="1">
+        <v>44273</v>
+      </c>
+      <c r="C1303">
+        <v>10</v>
+      </c>
+      <c r="D1303">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1304" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1304" s="1">
+        <v>44274</v>
+      </c>
+      <c r="C1304">
+        <v>7</v>
+      </c>
+      <c r="D1304">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1305" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1305" s="1">
+        <v>44275</v>
+      </c>
+      <c r="C1305">
+        <v>4</v>
+      </c>
+      <c r="D1305">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1306" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1306" s="1">
+        <v>43547</v>
+      </c>
+      <c r="C1306">
+        <v>95</v>
+      </c>
+      <c r="D1306">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1307" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1307" s="1">
+        <v>43548</v>
+      </c>
+      <c r="C1307">
+        <v>85</v>
+      </c>
+      <c r="D1307">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1308" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1308" s="1">
+        <v>43549</v>
+      </c>
+      <c r="C1308">
+        <v>84</v>
+      </c>
+      <c r="D1308">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1309" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1309" s="1">
+        <v>43550</v>
+      </c>
+      <c r="C1309">
+        <v>80</v>
+      </c>
+      <c r="D1309">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1310" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1310" s="1">
+        <v>43551</v>
+      </c>
+      <c r="C1310">
+        <v>65</v>
+      </c>
+      <c r="D1310">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1311" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1311" s="1">
+        <v>43552</v>
+      </c>
+      <c r="C1311">
+        <v>50</v>
+      </c>
+      <c r="D1311">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1312" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1312" s="1">
+        <v>43553</v>
+      </c>
+      <c r="C1312">
+        <v>30</v>
+      </c>
+      <c r="D1312">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1313" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1313" s="1">
+        <v>43554</v>
+      </c>
+      <c r="C1313">
+        <v>15</v>
+      </c>
+      <c r="D1313">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1314" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1314" s="1">
+        <v>43556</v>
+      </c>
+      <c r="C1314">
+        <v>10</v>
+      </c>
+      <c r="D1314">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1315" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1315" s="1">
+        <v>43557</v>
+      </c>
+      <c r="C1315">
+        <v>5</v>
+      </c>
+      <c r="D1315">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1316" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1316" s="1">
+        <v>44673</v>
+      </c>
+      <c r="C1316">
+        <v>100</v>
+      </c>
+      <c r="D1316">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1317" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1317" s="1">
+        <v>44674</v>
+      </c>
+      <c r="C1317">
+        <v>99</v>
+      </c>
+      <c r="D1317">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1318" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1318" s="1">
+        <v>44675</v>
+      </c>
+      <c r="C1318">
+        <v>98</v>
+      </c>
+      <c r="D1318">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1319" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1319" s="1">
+        <v>44676</v>
+      </c>
+      <c r="C1319">
+        <v>97</v>
+      </c>
+      <c r="D1319">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1320" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1320" s="1">
+        <v>44677</v>
+      </c>
+      <c r="C1320">
+        <v>96</v>
+      </c>
+      <c r="D1320">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1321" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1321" s="1">
+        <v>44678</v>
+      </c>
+      <c r="C1321">
+        <v>94</v>
+      </c>
+      <c r="D1321">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1322" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1322" s="1">
+        <v>44679</v>
+      </c>
+      <c r="C1322">
+        <v>90</v>
+      </c>
+      <c r="D1322">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1323" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1323" s="1">
+        <v>44680</v>
+      </c>
+      <c r="C1323">
+        <v>80</v>
+      </c>
+      <c r="D1323">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1324" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1324" s="1">
+        <v>44681</v>
+      </c>
+      <c r="C1324">
+        <v>65</v>
+      </c>
+      <c r="D1324">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1325" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1325" s="1">
+        <v>44682</v>
+      </c>
+      <c r="C1325">
+        <v>60</v>
+      </c>
+      <c r="D1325">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1326" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1326" s="1">
+        <v>44683</v>
+      </c>
+      <c r="C1326">
+        <v>50</v>
+      </c>
+      <c r="D1326">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1327" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1327" s="1">
+        <v>44684</v>
+      </c>
+      <c r="C1327">
+        <v>50</v>
+      </c>
+      <c r="D1327">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1328" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1328" s="1">
+        <v>44685</v>
+      </c>
+      <c r="C1328">
+        <v>35</v>
+      </c>
+      <c r="D1328">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1329" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1329" s="1">
+        <v>44686</v>
+      </c>
+      <c r="C1329">
+        <v>20</v>
+      </c>
+      <c r="D1329">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1330" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1330" s="1">
+        <v>44687</v>
+      </c>
+      <c r="C1330">
+        <v>8</v>
+      </c>
+      <c r="D1330">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1331" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1331" s="1">
+        <v>44688</v>
+      </c>
+      <c r="C1331">
+        <v>5</v>
+      </c>
+      <c r="D1331">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1332" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1332" s="1">
+        <v>44287</v>
+      </c>
+      <c r="C1332">
+        <v>100</v>
+      </c>
+      <c r="D1332">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1333" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1333" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C1333">
+        <v>99</v>
+      </c>
+      <c r="D1333">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1334" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1334" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C1334">
+        <v>98</v>
+      </c>
+      <c r="D1334">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1335" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1335" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C1335">
+        <v>96</v>
+      </c>
+      <c r="D1335">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1336" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1336" s="1">
+        <v>44291</v>
+      </c>
+      <c r="C1336">
+        <v>94</v>
+      </c>
+      <c r="D1336">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1337" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1337" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C1337">
+        <v>90</v>
+      </c>
+      <c r="D1337">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1338" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1338" s="1">
+        <v>44293</v>
+      </c>
+      <c r="C1338">
+        <v>75</v>
+      </c>
+      <c r="D1338">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1339" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1339" s="1">
+        <v>44294</v>
+      </c>
+      <c r="C1339">
+        <v>60</v>
+      </c>
+      <c r="D1339">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1340" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1340" s="1">
+        <v>44295</v>
+      </c>
+      <c r="C1340">
+        <v>54</v>
+      </c>
+      <c r="D1340">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1341" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1341" s="1">
+        <v>44296</v>
+      </c>
+      <c r="C1341">
+        <v>45</v>
+      </c>
+      <c r="D1341">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1342" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1342" s="1">
+        <v>44299</v>
+      </c>
+      <c r="C1342">
+        <v>44</v>
+      </c>
+      <c r="D1342">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1343" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1343" s="1">
+        <v>44300</v>
+      </c>
+      <c r="C1343">
+        <v>35</v>
+      </c>
+      <c r="D1343">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1344" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1344" s="1">
+        <v>44301</v>
+      </c>
+      <c r="C1344">
+        <v>20</v>
+      </c>
+      <c r="D1344">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1345" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1345" s="1">
+        <v>44302</v>
+      </c>
+      <c r="C1345">
+        <v>15</v>
+      </c>
+      <c r="D1345">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1346" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1346" s="1">
+        <v>44303</v>
+      </c>
+      <c r="C1346">
+        <v>10</v>
+      </c>
+      <c r="D1346">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1347" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1347" s="1">
+        <v>43944</v>
+      </c>
+      <c r="C1347">
+        <v>95</v>
+      </c>
+      <c r="D1347">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1348" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1348" s="1">
+        <v>43945</v>
+      </c>
+      <c r="C1348">
+        <v>90</v>
+      </c>
+      <c r="D1348">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1349" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1349" s="1">
+        <v>43946</v>
+      </c>
+      <c r="C1349">
+        <v>75</v>
+      </c>
+      <c r="D1349">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1350" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1350" s="1">
+        <v>43947</v>
+      </c>
+      <c r="C1350">
+        <v>35</v>
+      </c>
+      <c r="D1350">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1351" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1351" s="1">
+        <v>43948</v>
+      </c>
+      <c r="C1351">
+        <v>15</v>
+      </c>
+      <c r="D1351">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1352" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1352" s="1">
+        <v>43949</v>
+      </c>
+      <c r="C1352">
+        <v>5</v>
+      </c>
+      <c r="D1352">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1353" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1353" s="1">
+        <v>43566</v>
+      </c>
+      <c r="C1353">
+        <v>97</v>
+      </c>
+      <c r="D1353">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1354" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1354" s="1">
+        <v>43567</v>
+      </c>
+      <c r="C1354">
+        <v>95</v>
+      </c>
+      <c r="D1354">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1355" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1355" s="1">
+        <v>43568</v>
+      </c>
+      <c r="C1355">
+        <v>90</v>
+      </c>
+      <c r="D1355">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1356" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1356" s="1">
+        <v>43569</v>
+      </c>
+      <c r="C1356">
+        <v>87</v>
+      </c>
+      <c r="D1356">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1357" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1357" s="1">
+        <v>43570</v>
+      </c>
+      <c r="C1357">
+        <v>85</v>
+      </c>
+      <c r="D1357">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1358" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1358" s="1">
+        <v>43571</v>
+      </c>
+      <c r="C1358">
+        <v>73</v>
+      </c>
+      <c r="D1358">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1359" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1359" s="1">
+        <v>43572</v>
+      </c>
+      <c r="C1359">
+        <v>60</v>
+      </c>
+      <c r="D1359">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1360" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1360" s="1">
+        <v>43573</v>
+      </c>
+      <c r="C1360">
+        <v>33</v>
+      </c>
+      <c r="D1360">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1361" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1361" s="1">
+        <v>43574</v>
+      </c>
+      <c r="C1361">
+        <v>20</v>
+      </c>
+      <c r="D1361">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1362" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1362" s="1">
+        <v>43575</v>
+      </c>
+      <c r="C1362">
+        <v>10</v>
+      </c>
+      <c r="D1362">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1363" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1363" s="1">
+        <v>43576</v>
+      </c>
+      <c r="C1363">
+        <v>7</v>
+      </c>
+      <c r="D1363">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1364" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1364" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C1364">
+        <v>4</v>
+      </c>
+      <c r="D1364">
+        <v>2019</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added classifications for all sites, we move on
</commit_message>
<xml_diff>
--- a/snow_timeline.xlsx
+++ b/snow_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1803229\Documents\Snowstradamus\Snowstradamus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6F897A-47C1-43EE-B553-ADC0740AD5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2155AB-61F6-4A97-9D90-55D570FA8EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5868" yWindow="-72" windowWidth="17280" windowHeight="9960" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
+    <workbookView xWindow="5856" yWindow="0" windowWidth="17280" windowHeight="9960" xr2:uid="{C4BA0D95-1C30-456C-B2BA-46850E4E26C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="22">
   <si>
     <t>Location</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>hyytiala</t>
+  </si>
+  <si>
+    <t>tammela</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0BDC52-0678-4879-BFA4-045E88D6C76C}">
-  <dimension ref="A1:D1262"/>
+  <dimension ref="A1:D1277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1230" workbookViewId="0">
-      <selection activeCell="C1257" sqref="C1257"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="E372" sqref="E372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18116,49 +18119,325 @@
       </c>
     </row>
     <row r="1255" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1255" t="s">
+        <v>20</v>
+      </c>
       <c r="B1255" s="1">
         <v>43571</v>
       </c>
       <c r="C1255">
         <v>97</v>
       </c>
+      <c r="D1255">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1256" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1256" t="s">
+        <v>20</v>
+      </c>
       <c r="B1256" s="1">
         <v>43572</v>
       </c>
       <c r="C1256">
         <v>95</v>
       </c>
+      <c r="D1256">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1257" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1257" t="s">
+        <v>20</v>
+      </c>
       <c r="B1257" s="1">
         <v>43573</v>
       </c>
+      <c r="C1257">
+        <v>90</v>
+      </c>
+      <c r="D1257">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1258" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1258" t="s">
+        <v>20</v>
+      </c>
       <c r="B1258" s="1">
         <v>43574</v>
       </c>
+      <c r="C1258">
+        <v>80</v>
+      </c>
+      <c r="D1258">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1259" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1259" t="s">
+        <v>20</v>
+      </c>
       <c r="B1259" s="1">
         <v>43575</v>
       </c>
+      <c r="C1259">
+        <v>65</v>
+      </c>
+      <c r="D1259">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1260" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1260" t="s">
+        <v>20</v>
+      </c>
       <c r="B1260" s="1">
         <v>43576</v>
       </c>
+      <c r="C1260">
+        <v>45</v>
+      </c>
+      <c r="D1260">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1261" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1261" t="s">
+        <v>20</v>
+      </c>
       <c r="B1261" s="1">
         <v>43577</v>
       </c>
+      <c r="C1261">
+        <v>15</v>
+      </c>
+      <c r="D1261">
+        <v>2019</v>
+      </c>
     </row>
     <row r="1262" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1262" t="s">
+        <v>20</v>
+      </c>
       <c r="B1262" s="1">
         <v>43578</v>
+      </c>
+      <c r="C1262">
+        <v>8</v>
+      </c>
+      <c r="D1262">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1263" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1263" s="1">
+        <v>43579</v>
+      </c>
+      <c r="C1263">
+        <v>3</v>
+      </c>
+      <c r="D1263">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1264" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1264" s="1">
+        <v>44667</v>
+      </c>
+      <c r="C1264">
+        <v>99</v>
+      </c>
+      <c r="D1264">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1265" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1265" s="1">
+        <v>44668</v>
+      </c>
+      <c r="C1265">
+        <v>98.5</v>
+      </c>
+      <c r="D1265">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1266" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1266" s="1">
+        <v>44669</v>
+      </c>
+      <c r="C1266">
+        <v>98</v>
+      </c>
+      <c r="D1266">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1267" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1267" s="1">
+        <v>44671</v>
+      </c>
+      <c r="C1267">
+        <v>80</v>
+      </c>
+      <c r="D1267">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1268" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1268" s="1">
+        <v>44672</v>
+      </c>
+      <c r="C1268">
+        <v>30</v>
+      </c>
+      <c r="D1268">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1269" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1269" s="1">
+        <v>44673</v>
+      </c>
+      <c r="C1269">
+        <v>10</v>
+      </c>
+      <c r="D1269">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1270" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1270" s="1">
+        <v>44279</v>
+      </c>
+      <c r="C1270">
+        <v>99</v>
+      </c>
+      <c r="D1270">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1271" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1271" s="1">
+        <v>44284</v>
+      </c>
+      <c r="C1271">
+        <v>90</v>
+      </c>
+      <c r="D1271">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1272" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1272" s="1">
+        <v>44285</v>
+      </c>
+      <c r="C1272">
+        <v>70</v>
+      </c>
+      <c r="D1272">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1273" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1273" s="1">
+        <v>44286</v>
+      </c>
+      <c r="C1273">
+        <v>45</v>
+      </c>
+      <c r="D1273">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1274" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1274" s="1">
+        <v>44287</v>
+      </c>
+      <c r="C1274">
+        <v>25</v>
+      </c>
+      <c r="D1274">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1275" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1275" s="1">
+        <v>44288</v>
+      </c>
+      <c r="C1275">
+        <v>15</v>
+      </c>
+      <c r="D1275">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1276" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1276" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C1276">
+        <v>10</v>
+      </c>
+      <c r="D1276">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1277" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1277" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C1277">
+        <v>5</v>
+      </c>
+      <c r="D1277">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>